<commit_message>
partizione raccolte per settimana
</commit_message>
<xml_diff>
--- a/backend/doc_templates/report.xlsx
+++ b/backend/doc_templates/report.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="127">
   <si>
     <t xml:space="preserve"> PRODUZIONE RIFIUTI - IMBALLAGGI VUOTATI  </t>
   </si>
@@ -146,6 +146,141 @@
     <t xml:space="preserve">PRODUZIONE</t>
   </si>
   <si>
+    <t xml:space="preserve">TOTALE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DA SMALTIRE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DATA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">       SMALTITO </t>
+  </si>
+  <si>
+    <t xml:space="preserve">STOCK FINALE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CALCOLO DEL PESO NETTO TEORICO  PER LA  COMPILAZIONE DEL FORMULARIO E ANCORA  PRIMA DELLA REGISTRAZIONE MOVIMENTO IN AD-HOC </t>
+  </si>
+  <si>
+    <t xml:space="preserve">tara Kg/pz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kg       SMALTITI </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> PRODUZIONE - RIFIUTI NON PERICOLOSI - REPARTO PRODUZIONE  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">MOD 22 A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12-05-2024     Rev. 07</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SOSTANZE NON PERICOLOSE        -       CER 16.03.06</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RIFIUTI NON PERICOLOSI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Materia prima e prodotti fuori specifica  contenuti in imballaggi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CER 16.02.14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CER 17.04.07</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CER 16.03.04</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CER 16.10.02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PLASTICI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">METALLICI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DI MATERIALI MISTI           </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ELLETTRICI             RAE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">METALLI MISTI </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RIFIUTI INORGANICI  NON PERICOLOSI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Soluzioni acquose di scarto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sacche</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fusti FP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fustini</t>
+  </si>
+  <si>
+    <t xml:space="preserve">secchie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">taniche</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fusti FF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">secchielli</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cisterne</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fusti cart</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Smartphone, PC, stampanti, fotocopiatrici, router, mouse</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ferro, acciaio, rame, ottone</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Plast-Fe-legno</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cartone-plastic - Fe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sale marino</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Acqua lavaggio pavimenti</t>
+  </si>
+  <si>
+    <t xml:space="preserve">esistenze</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kg Netti</t>
+  </si>
+  <si>
+    <t xml:space="preserve">inizio periodo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">in Pezzi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PRODUZIONE RIFIUTI</t>
+  </si>
+  <si>
     <t xml:space="preserve">Sett-36</t>
   </si>
   <si>
@@ -156,141 +291,6 @@
   </si>
   <si>
     <t xml:space="preserve">Sett-39</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TOTALE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DA SMALTIRE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DATA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">       SMALTITO </t>
-  </si>
-  <si>
-    <t xml:space="preserve">STOCK FINALE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CALCOLO DEL PESO NETTO TEORICO  PER LA  COMPILAZIONE DEL FORMULARIO E ANCORA  PRIMA DELLA REGISTRAZIONE MOVIMENTO IN AD-HOC </t>
-  </si>
-  <si>
-    <t xml:space="preserve">tara Kg/pz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kg       SMALTITI </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> PRODUZIONE - RIFIUTI NON PERICOLOSI - REPARTO PRODUZIONE  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">MOD 22 A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">12-05-2024     Rev. 07</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SOSTANZE NON PERICOLOSE        -       CER 16.03.06</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RIFIUTI NON PERICOLOSI</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Materia prima e prodotti fuori specifica  contenuti in imballaggi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CER 16.02.14</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CER 17.04.07</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CER 16.03.04</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CER 16.10.02</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PLASTICI</t>
-  </si>
-  <si>
-    <t xml:space="preserve">METALLICI</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DI MATERIALI MISTI           </t>
-  </si>
-  <si>
-    <t xml:space="preserve">ELLETTRICI             RAE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">METALLI MISTI </t>
-  </si>
-  <si>
-    <t xml:space="preserve">RIFIUTI INORGANICI  NON PERICOLOSI</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Soluzioni acquose di scarto</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sacche</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fusti FP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fustini</t>
-  </si>
-  <si>
-    <t xml:space="preserve">secchie</t>
-  </si>
-  <si>
-    <t xml:space="preserve">taniche</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fusti FF</t>
-  </si>
-  <si>
-    <t xml:space="preserve">secchielli</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cisterne</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fusti cart</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Smartphone, PC, stampanti, fotocopiatrici, router, mouse</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ferro, acciaio, rame, ottone</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Plast-Fe-legno</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cartone-plastic - Fe</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sale marino</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Acqua lavaggio pavimenti</t>
-  </si>
-  <si>
-    <t xml:space="preserve">esistenze</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kg Netti</t>
-  </si>
-  <si>
-    <t xml:space="preserve">inizio periodo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">in Pezzi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PRODUZIONE RIFIUTI</t>
   </si>
   <si>
     <t xml:space="preserve">prodotto al </t>
@@ -3401,9 +3401,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>114120</xdr:colOff>
+      <xdr:colOff>113760</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>289440</xdr:rowOff>
+      <xdr:rowOff>289080</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3417,7 +3417,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="658080" y="23040"/>
-          <a:ext cx="1572480" cy="809280"/>
+          <a:ext cx="1571400" cy="808920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3443,9 +3443,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>761760</xdr:colOff>
+      <xdr:colOff>761400</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>209520</xdr:rowOff>
+      <xdr:rowOff>209160</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3458,8 +3458,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="703440" y="23040"/>
-          <a:ext cx="2379240" cy="681840"/>
+          <a:off x="704160" y="23040"/>
+          <a:ext cx="2378880" cy="681480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3485,9 +3485,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>616680</xdr:colOff>
+      <xdr:colOff>616320</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>274680</xdr:rowOff>
+      <xdr:rowOff>274320</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3500,8 +3500,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1544040" y="23040"/>
-          <a:ext cx="2193120" cy="747000"/>
+          <a:off x="1544760" y="23040"/>
+          <a:ext cx="2192760" cy="746640"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3526,13 +3526,13 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="G15" activeCellId="0" sqref="G15"/>
+      <selection pane="bottomLeft" activeCell="C19" activeCellId="0" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="8.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.2"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="11.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="12" style="0" width="8.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="11.77"/>
@@ -3890,9 +3890,7 @@
       <c r="B13" s="67" t="s">
         <v>38</v>
       </c>
-      <c r="C13" s="68" t="s">
-        <v>39</v>
-      </c>
+      <c r="C13" s="68"/>
       <c r="D13" s="69"/>
       <c r="E13" s="70"/>
       <c r="F13" s="71"/>
@@ -3932,9 +3930,7 @@
     </row>
     <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B15" s="67"/>
-      <c r="C15" s="85" t="s">
-        <v>40</v>
-      </c>
+      <c r="C15" s="85"/>
       <c r="D15" s="86"/>
       <c r="E15" s="87"/>
       <c r="F15" s="88"/>
@@ -3974,9 +3970,7 @@
     </row>
     <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B17" s="67"/>
-      <c r="C17" s="94" t="s">
-        <v>41</v>
-      </c>
+      <c r="C17" s="94"/>
       <c r="D17" s="95"/>
       <c r="E17" s="82"/>
       <c r="F17" s="96"/>
@@ -4016,9 +4010,7 @@
     </row>
     <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B19" s="67"/>
-      <c r="C19" s="85" t="s">
-        <v>42</v>
-      </c>
+      <c r="C19" s="85"/>
       <c r="D19" s="95"/>
       <c r="E19" s="87"/>
       <c r="F19" s="88"/>
@@ -4118,7 +4110,7 @@
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B24" s="118" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C24" s="119" t="s">
         <v>36</v>
@@ -4229,7 +4221,7 @@
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B27" s="138" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C27" s="119" t="s">
         <v>36</v>
@@ -4321,7 +4313,7 @@
     <row r="29" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B29" s="1"/>
       <c r="C29" s="143" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D29" s="114"/>
       <c r="E29" s="114"/>
@@ -4342,7 +4334,7 @@
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B30" s="144" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C30" s="145"/>
       <c r="D30" s="146"/>
@@ -4444,7 +4436,7 @@
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B35" s="46" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C35" s="119" t="s">
         <v>36</v>
@@ -4558,7 +4550,7 @@
     <row r="38" customFormat="false" ht="33" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="186"/>
       <c r="B38" s="187" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C38" s="187"/>
       <c r="D38" s="187"/>
@@ -4584,7 +4576,7 @@
       <c r="A39" s="186"/>
       <c r="B39" s="186"/>
       <c r="C39" s="188" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="D39" s="189" t="n">
         <v>10</v>
@@ -4710,7 +4702,7 @@
     <row r="42" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="186"/>
       <c r="B42" s="198" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C42" s="199" t="n">
         <f aca="false">+C30</f>
@@ -5100,7 +5092,7 @@
       <selection pane="bottomRight" activeCell="I12" activeCellId="0" sqref="I12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="11.33"/>
@@ -5118,7 +5110,7 @@
       <c r="C1" s="227"/>
       <c r="D1" s="228"/>
       <c r="E1" s="229" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="F1" s="229"/>
       <c r="G1" s="229"/>
@@ -5132,7 +5124,7 @@
       <c r="O1" s="229"/>
       <c r="P1" s="229"/>
       <c r="Q1" s="5" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="R1" s="5"/>
       <c r="S1" s="230"/>
@@ -5166,7 +5158,7 @@
       </c>
       <c r="P2" s="15"/>
       <c r="Q2" s="16" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="R2" s="16"/>
       <c r="S2" s="234"/>
@@ -5214,7 +5206,7 @@
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="237" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="E4" s="237"/>
       <c r="F4" s="237"/>
@@ -5227,7 +5219,7 @@
       <c r="M4" s="237"/>
       <c r="N4" s="237"/>
       <c r="O4" s="238" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="P4" s="238"/>
       <c r="Q4" s="238"/>
@@ -5243,7 +5235,7 @@
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="239" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="E5" s="239"/>
       <c r="F5" s="239"/>
@@ -5256,16 +5248,16 @@
       <c r="M5" s="239"/>
       <c r="N5" s="239"/>
       <c r="O5" s="240" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="P5" s="241" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="Q5" s="242" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="R5" s="241" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="S5" s="1"/>
       <c r="T5" s="1"/>
@@ -5278,33 +5270,33 @@
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="243" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="E6" s="243"/>
       <c r="F6" s="243"/>
       <c r="G6" s="243"/>
       <c r="H6" s="243"/>
       <c r="I6" s="244" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="J6" s="244"/>
       <c r="K6" s="244"/>
       <c r="L6" s="244"/>
       <c r="M6" s="245" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="N6" s="245"/>
       <c r="O6" s="246" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="P6" s="246" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="Q6" s="247" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="R6" s="247" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="S6" s="1"/>
       <c r="T6" s="1"/>
@@ -5342,41 +5334,41 @@
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="248" t="s">
+        <v>64</v>
+      </c>
+      <c r="E8" s="249" t="s">
+        <v>65</v>
+      </c>
+      <c r="F8" s="250" t="s">
+        <v>66</v>
+      </c>
+      <c r="G8" s="249" t="s">
+        <v>67</v>
+      </c>
+      <c r="H8" s="251" t="s">
         <v>68</v>
-      </c>
-      <c r="E8" s="249" t="s">
-        <v>69</v>
-      </c>
-      <c r="F8" s="250" t="s">
-        <v>70</v>
-      </c>
-      <c r="G8" s="249" t="s">
-        <v>71</v>
-      </c>
-      <c r="H8" s="251" t="s">
-        <v>72</v>
       </c>
       <c r="I8" s="248"/>
       <c r="J8" s="249" t="s">
+        <v>69</v>
+      </c>
+      <c r="K8" s="250" t="s">
+        <v>67</v>
+      </c>
+      <c r="L8" s="252" t="s">
+        <v>70</v>
+      </c>
+      <c r="M8" s="248" t="s">
+        <v>71</v>
+      </c>
+      <c r="N8" s="253" t="s">
+        <v>72</v>
+      </c>
+      <c r="O8" s="254" t="s">
         <v>73</v>
       </c>
-      <c r="K8" s="250" t="s">
-        <v>71</v>
-      </c>
-      <c r="L8" s="252" t="s">
+      <c r="P8" s="254" t="s">
         <v>74</v>
-      </c>
-      <c r="M8" s="248" t="s">
-        <v>75</v>
-      </c>
-      <c r="N8" s="253" t="s">
-        <v>76</v>
-      </c>
-      <c r="O8" s="254" t="s">
-        <v>77</v>
-      </c>
-      <c r="P8" s="254" t="s">
-        <v>78</v>
       </c>
       <c r="Q8" s="247"/>
       <c r="R8" s="247"/>
@@ -5400,18 +5392,18 @@
       <c r="K9" s="258"/>
       <c r="L9" s="260"/>
       <c r="M9" s="261" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="N9" s="262" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="O9" s="254"/>
       <c r="P9" s="254"/>
       <c r="Q9" s="263" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="R9" s="263" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="S9" s="1"/>
       <c r="T9" s="1"/>
@@ -5472,10 +5464,10 @@
     <row r="12" customFormat="false" ht="27.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="1"/>
       <c r="B12" s="272" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C12" s="273" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D12" s="274"/>
       <c r="E12" s="275"/>
@@ -5497,10 +5489,10 @@
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="1"/>
       <c r="B13" s="280" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C13" s="281" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D13" s="282"/>
       <c r="E13" s="283"/>
@@ -5522,10 +5514,10 @@
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="1"/>
       <c r="B14" s="289" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C14" s="68" t="s">
-        <v>39</v>
+        <v>84</v>
       </c>
       <c r="D14" s="290"/>
       <c r="E14" s="291"/>
@@ -5569,7 +5561,7 @@
       <c r="A16" s="1"/>
       <c r="B16" s="289"/>
       <c r="C16" s="85" t="s">
-        <v>40</v>
+        <v>85</v>
       </c>
       <c r="D16" s="303"/>
       <c r="E16" s="291"/>
@@ -5613,7 +5605,7 @@
       <c r="A18" s="1"/>
       <c r="B18" s="289"/>
       <c r="C18" s="94" t="s">
-        <v>41</v>
+        <v>86</v>
       </c>
       <c r="D18" s="303"/>
       <c r="E18" s="291"/>
@@ -5657,7 +5649,7 @@
       <c r="A20" s="1"/>
       <c r="B20" s="289"/>
       <c r="C20" s="85" t="s">
-        <v>42</v>
+        <v>87</v>
       </c>
       <c r="D20" s="303"/>
       <c r="E20" s="291"/>
@@ -5837,7 +5829,7 @@
       <c r="A26" s="1"/>
       <c r="B26" s="329"/>
       <c r="C26" s="322" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D26" s="214"/>
       <c r="E26" s="330"/>
@@ -5955,7 +5947,7 @@
       <c r="A29" s="1"/>
       <c r="B29" s="339"/>
       <c r="C29" s="322" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D29" s="340" t="n">
         <f aca="false">+D13+D26</f>
@@ -6065,7 +6057,7 @@
         <v>45426</v>
       </c>
       <c r="C32" s="322" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D32" s="346"/>
       <c r="E32" s="347"/>
@@ -6186,7 +6178,7 @@
         <v>95</v>
       </c>
       <c r="C35" s="322" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D35" s="323" t="n">
         <f aca="false">+D29-D32</f>
@@ -6393,7 +6385,7 @@
       <selection pane="topLeft" activeCell="M38" activeCellId="0" sqref="M38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="11.33"/>
@@ -6466,7 +6458,7 @@
       <c r="R2" s="8"/>
       <c r="S2" s="358"/>
       <c r="T2" s="16" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="U2" s="16"/>
       <c r="V2" s="16"/>
@@ -6676,10 +6668,10 @@
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="376" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="E9" s="377" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="F9" s="378" t="s">
         <v>119</v>
@@ -6711,43 +6703,43 @@
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="381" t="s">
+        <v>65</v>
+      </c>
+      <c r="E10" s="382" t="s">
         <v>69</v>
       </c>
-      <c r="E10" s="382" t="s">
-        <v>73</v>
-      </c>
       <c r="F10" s="383" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="G10" s="384" t="s">
+        <v>64</v>
+      </c>
+      <c r="H10" s="249" t="s">
+        <v>65</v>
+      </c>
+      <c r="I10" s="250" t="s">
+        <v>66</v>
+      </c>
+      <c r="J10" s="249" t="s">
+        <v>67</v>
+      </c>
+      <c r="K10" s="251" t="s">
         <v>68</v>
       </c>
-      <c r="H10" s="249" t="s">
+      <c r="L10" s="248" t="s">
         <v>69</v>
       </c>
-      <c r="I10" s="250" t="s">
-        <v>70</v>
-      </c>
-      <c r="J10" s="249" t="s">
-        <v>71</v>
-      </c>
-      <c r="K10" s="251" t="s">
-        <v>72</v>
-      </c>
-      <c r="L10" s="248" t="s">
-        <v>73</v>
-      </c>
       <c r="M10" s="249" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="N10" s="250" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="O10" s="250" t="s">
         <v>122</v>
       </c>
       <c r="P10" s="385" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="Q10" s="386" t="s">
         <v>123</v>
@@ -6789,10 +6781,10 @@
     <row r="12" customFormat="false" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="1"/>
       <c r="B12" s="387" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C12" s="273" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D12" s="388"/>
       <c r="E12" s="276" t="n">
@@ -6822,10 +6814,10 @@
     <row r="13" customFormat="false" ht="32.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="1"/>
       <c r="B13" s="393" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C13" s="394" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D13" s="395"/>
       <c r="E13" s="285" t="n">
@@ -6855,10 +6847,10 @@
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="1"/>
       <c r="B14" s="399" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C14" s="68" t="s">
-        <v>39</v>
+        <v>84</v>
       </c>
       <c r="D14" s="294"/>
       <c r="E14" s="292" t="n">
@@ -6914,7 +6906,7 @@
       <c r="A16" s="1"/>
       <c r="B16" s="399"/>
       <c r="C16" s="85" t="s">
-        <v>40</v>
+        <v>85</v>
       </c>
       <c r="D16" s="292"/>
       <c r="E16" s="292"/>
@@ -6966,7 +6958,7 @@
       <c r="A18" s="1"/>
       <c r="B18" s="399"/>
       <c r="C18" s="94" t="s">
-        <v>41</v>
+        <v>86</v>
       </c>
       <c r="D18" s="292"/>
       <c r="E18" s="292"/>
@@ -7018,7 +7010,7 @@
       <c r="A20" s="1"/>
       <c r="B20" s="399"/>
       <c r="C20" s="85" t="s">
-        <v>42</v>
+        <v>87</v>
       </c>
       <c r="D20" s="292"/>
       <c r="E20" s="292"/>
@@ -7231,7 +7223,7 @@
       <c r="A26" s="1"/>
       <c r="B26" s="329"/>
       <c r="C26" s="322" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D26" s="411"/>
       <c r="E26" s="218" t="n">
@@ -7376,7 +7368,7 @@
       <c r="A29" s="1"/>
       <c r="B29" s="339"/>
       <c r="C29" s="322" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D29" s="324" t="n">
         <f aca="false">+D13+D26</f>
@@ -7503,7 +7495,7 @@
       <c r="A32" s="1"/>
       <c r="B32" s="345"/>
       <c r="C32" s="322" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D32" s="421"/>
       <c r="E32" s="422"/>
@@ -7645,7 +7637,7 @@
         <v>95</v>
       </c>
       <c r="C35" s="322" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D35" s="431" t="n">
         <f aca="false">+D29-D32</f>

</xml_diff>